<commit_message>
Added Version 10 of code, updated notes, and optimization metrics spreadsheet
</commit_message>
<xml_diff>
--- a/Alex/Optimization_Metrics.xlsx
+++ b/Alex/Optimization_Metrics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asg_a_1p8y6mm\Downloads\Project_04\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{113DC2C6-5F43-4759-BB2F-E5BAF71FF34E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44777F81-8434-4564-A085-893BF29E491A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{6E00537D-A3CB-4DE7-973B-44E1FD35F5BD}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
   <si>
     <t>Accuracy</t>
   </si>
@@ -94,6 +94,18 @@
   </si>
   <si>
     <t>Logistic Regression 9 (Add Calibration Curve and Odds Ratio to analyze linear regression)</t>
+  </si>
+  <si>
+    <t>Model Metric</t>
+  </si>
+  <si>
+    <t>Logistic Regression</t>
+  </si>
+  <si>
+    <t>Random Forest</t>
+  </si>
+  <si>
+    <t>Logistic Regression 10 (Optimize Random Forest)</t>
   </si>
 </sst>
 </file>
@@ -101,7 +113,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -146,7 +158,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -399,38 +411,152 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
@@ -440,6 +566,22 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -754,230 +896,307 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDBE8DC2-E395-4175-AFF2-1F4BE9386154}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="81.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="8.7265625" style="2"/>
-    <col min="8" max="8" width="24.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.453125" customWidth="1"/>
+    <col min="3" max="7" width="8.7265625" style="2"/>
+    <col min="9" max="9" width="24.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="D1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="E1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="F1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="G1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="I1" s="20" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="15" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="16">
+      <c r="B2" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="13">
         <v>0.86704999999999999</v>
       </c>
-      <c r="C2" s="16">
+      <c r="D2" s="13">
         <v>0.83450800000000003</v>
       </c>
-      <c r="D2" s="16">
+      <c r="E2" s="13">
         <v>0.86704999999999999</v>
       </c>
-      <c r="E2" s="16">
+      <c r="F2" s="13">
         <v>0.83391899999999997</v>
       </c>
-      <c r="F2" s="17">
+      <c r="G2" s="14">
         <v>0.82298400000000005</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="I2" s="19" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="3">
         <v>0.86704999999999999</v>
       </c>
-      <c r="C3" s="3">
+      <c r="D3" s="3">
         <v>0.83450800000000003</v>
       </c>
-      <c r="D3" s="3">
+      <c r="E3" s="3">
         <v>0.86704999999999999</v>
       </c>
-      <c r="E3" s="3">
+      <c r="F3" s="3">
         <v>0.83391899999999997</v>
       </c>
-      <c r="F3" s="8">
+      <c r="G3" s="8">
         <v>0.82298400000000005</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="I3" s="18" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="4">
         <v>0.86752300000000004</v>
       </c>
-      <c r="C4" s="4">
+      <c r="D4" s="4">
         <v>0.83518300000000001</v>
       </c>
-      <c r="D4" s="4">
+      <c r="E4" s="4">
         <v>0.86752300000000004</v>
       </c>
-      <c r="E4" s="5">
+      <c r="F4" s="5">
         <v>0.83322099999999999</v>
       </c>
-      <c r="F4" s="9">
+      <c r="G4" s="9">
         <v>0.82414200000000004</v>
       </c>
-      <c r="H4" s="25" t="s">
+      <c r="I4" s="22" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="3">
         <v>0.86752300000000004</v>
       </c>
-      <c r="C5" s="5">
+      <c r="D5" s="5">
         <v>0.83514699999999997</v>
       </c>
-      <c r="D5" s="3">
+      <c r="E5" s="3">
         <v>0.86752300000000004</v>
       </c>
-      <c r="E5" s="5">
+      <c r="F5" s="5">
         <v>0.83307200000000003</v>
       </c>
-      <c r="F5" s="10">
+      <c r="G5" s="10">
         <v>0.82414399999999999</v>
       </c>
-      <c r="H5" s="24" t="s">
+      <c r="I5" s="21" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="5">
         <v>0.86739200000000005</v>
       </c>
-      <c r="C6" s="4">
+      <c r="D6" s="4">
         <v>0.835368</v>
       </c>
-      <c r="D6" s="5">
+      <c r="E6" s="5">
         <v>0.86739200000000005</v>
       </c>
-      <c r="E6" s="4">
+      <c r="F6" s="4">
         <v>0.83470599999999995</v>
       </c>
-      <c r="F6" s="11">
+      <c r="G6" s="11">
         <v>0.82350000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="4">
         <v>0.86741800000000002</v>
       </c>
-      <c r="C7" s="4">
+      <c r="D7" s="4">
         <v>0.83543800000000001</v>
       </c>
-      <c r="D7" s="4">
+      <c r="E7" s="4">
         <v>0.86741800000000002</v>
       </c>
-      <c r="E7" s="6">
+      <c r="F7" s="6">
         <v>0.83478200000000002</v>
       </c>
-      <c r="F7" s="11">
+      <c r="G7" s="11">
         <v>0.82349300000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="6">
         <v>0.86744500000000002</v>
       </c>
-      <c r="C8" s="6">
+      <c r="D8" s="6">
         <v>0.83548100000000003</v>
       </c>
-      <c r="D8" s="6">
+      <c r="E8" s="6">
         <v>0.86744500000000002</v>
       </c>
-      <c r="E8" s="5">
+      <c r="F8" s="5">
         <v>0.83477199999999996</v>
       </c>
-      <c r="F8" s="8">
+      <c r="G8" s="8">
         <v>0.82349300000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="3">
         <v>0.86744500000000002</v>
       </c>
-      <c r="C9" s="3">
+      <c r="D9" s="3">
         <v>0.83548100000000003</v>
       </c>
-      <c r="D9" s="3">
+      <c r="E9" s="3">
         <v>0.86744500000000002</v>
       </c>
-      <c r="E9" s="3">
+      <c r="F9" s="3">
         <v>0.83477199999999996</v>
       </c>
-      <c r="F9" s="8">
+      <c r="G9" s="8">
         <v>0.82349300000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="12" t="s">
+    <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="13">
+      <c r="B10" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="27">
         <v>0.86744500000000002</v>
       </c>
-      <c r="C10" s="13">
+      <c r="D10" s="27">
         <v>0.83548100000000003</v>
       </c>
-      <c r="D10" s="13">
+      <c r="E10" s="27">
         <v>0.86744500000000002</v>
       </c>
-      <c r="E10" s="13">
+      <c r="F10" s="27">
         <v>0.83477199999999996</v>
       </c>
-      <c r="F10" s="14">
+      <c r="G10" s="28">
         <v>0.82349300000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="31">
+        <v>0.85821999999999998</v>
+      </c>
+      <c r="D11" s="31">
+        <v>0.82387299999999997</v>
+      </c>
+      <c r="E11" s="31">
+        <v>0.85821999999999998</v>
+      </c>
+      <c r="F11" s="31">
+        <v>0.83196300000000001</v>
+      </c>
+      <c r="G11" s="32">
+        <v>0.79233299999999995</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="33">
+        <v>0.86150499999999997</v>
+      </c>
+      <c r="D12" s="33">
+        <v>0.82802500000000001</v>
+      </c>
+      <c r="E12" s="33">
+        <v>0.86150499999999997</v>
+      </c>
+      <c r="F12" s="33">
+        <v>0.83425400000000005</v>
+      </c>
+      <c r="G12" s="36">
+        <v>0.80271800000000004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added eleventh and twelfth versions of Jupyter notebook which add Gradient Boost optimization, as well as optimization log spreadsheet and updated note file
</commit_message>
<xml_diff>
--- a/Alex/Optimization_Metrics.xlsx
+++ b/Alex/Optimization_Metrics.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asg_a_1p8y6mm\Downloads\Project_04\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44777F81-8434-4564-A085-893BF29E491A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECB0A5AD-654D-40DA-82EE-70D87E747AEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{6E00537D-A3CB-4DE7-973B-44E1FD35F5BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
   <si>
     <t>Accuracy</t>
   </si>
@@ -106,6 +107,24 @@
   </si>
   <si>
     <t>Logistic Regression 10 (Optimize Random Forest)</t>
+  </si>
+  <si>
+    <t>Gradient</t>
+  </si>
+  <si>
+    <t>Gradient Boosting</t>
+  </si>
+  <si>
+    <t>Logistic Regression 11 (Optimize Gradient Boosting)</t>
+  </si>
+  <si>
+    <t>Before</t>
+  </si>
+  <si>
+    <t>After</t>
+  </si>
+  <si>
+    <t>Logistic Regression 12 (Optimize Gradient Boosting; expanded with early stopping)</t>
   </si>
 </sst>
 </file>
@@ -115,7 +134,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,6 +149,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="5">
@@ -158,7 +182,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -528,11 +552,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -574,14 +620,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -896,11 +958,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDBE8DC2-E395-4175-AFF2-1F4BE9386154}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="81.36328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.453125" customWidth="1"/>
@@ -908,7 +970,7 @@
     <col min="9" max="9" width="24.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="15" thickBot="1">
       <c r="A1" s="15" t="s">
         <v>5</v>
       </c>
@@ -934,7 +996,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9">
       <c r="A2" s="12" t="s">
         <v>11</v>
       </c>
@@ -960,7 +1022,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9">
       <c r="A3" s="7" t="s">
         <v>12</v>
       </c>
@@ -986,7 +1048,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:9" ht="15" thickBot="1">
       <c r="A4" s="7" t="s">
         <v>13</v>
       </c>
@@ -1012,7 +1074,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:9" ht="15" thickBot="1">
       <c r="A5" s="7" t="s">
         <v>14</v>
       </c>
@@ -1038,7 +1100,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9">
       <c r="A6" s="7" t="s">
         <v>15</v>
       </c>
@@ -1061,7 +1123,7 @@
         <v>0.82350000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9">
       <c r="A7" s="7" t="s">
         <v>16</v>
       </c>
@@ -1084,7 +1146,7 @@
         <v>0.82349300000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9">
       <c r="A8" s="7" t="s">
         <v>17</v>
       </c>
@@ -1107,7 +1169,7 @@
         <v>0.82349300000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9">
       <c r="A9" s="7" t="s">
         <v>18</v>
       </c>
@@ -1130,7 +1192,7 @@
         <v>0.82349300000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:9" ht="15" thickBot="1">
       <c r="A10" s="25" t="s">
         <v>19</v>
       </c>
@@ -1153,7 +1215,7 @@
         <v>0.82349300000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9">
       <c r="A11" s="29" t="s">
         <v>19</v>
       </c>
@@ -1176,27 +1238,199 @@
         <v>0.79233299999999995</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="34" t="s">
+    <row r="12" spans="1:9" ht="15" thickBot="1">
+      <c r="A12" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="35" t="s">
+      <c r="B12" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="33">
+      <c r="C12" s="40">
         <v>0.86150499999999997</v>
       </c>
-      <c r="D12" s="33">
+      <c r="D12" s="40">
         <v>0.82802500000000001</v>
       </c>
-      <c r="E12" s="33">
+      <c r="E12" s="40">
         <v>0.86150499999999997</v>
       </c>
-      <c r="F12" s="33">
+      <c r="F12" s="40">
         <v>0.83425400000000005</v>
       </c>
-      <c r="G12" s="36">
+      <c r="G12" s="41">
         <v>0.80271800000000004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="45">
+        <v>0.86915299999999995</v>
+      </c>
+      <c r="D13" s="45">
+        <v>0.83932499999999999</v>
+      </c>
+      <c r="E13" s="45">
+        <v>0.86915299999999995</v>
+      </c>
+      <c r="F13" s="31">
+        <v>0.83770100000000003</v>
+      </c>
+      <c r="G13" s="32">
+        <v>0.82853900000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="5">
+        <v>0.86878500000000003</v>
+      </c>
+      <c r="D14" s="5">
+        <v>0.83852000000000004</v>
+      </c>
+      <c r="E14" s="5">
+        <v>0.86878500000000003</v>
+      </c>
+      <c r="F14" s="5">
+        <v>0.83710499999999999</v>
+      </c>
+      <c r="G14" s="49">
+        <v>0.82854099999999997</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15" thickBot="1">
+      <c r="A15" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="50">
+        <v>0.86902100000000004</v>
+      </c>
+      <c r="D15" s="50">
+        <v>0.83910099999999999</v>
+      </c>
+      <c r="E15" s="50">
+        <v>0.86902100000000004</v>
+      </c>
+      <c r="F15" s="33">
+        <v>0.83774599999999999</v>
+      </c>
+      <c r="G15" s="43">
+        <v>0.82778499999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="37"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA0E0689-5345-46E6-81C6-E91955650508}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15" thickBot="1">
+      <c r="A1" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="45">
+        <v>0.86915299999999995</v>
+      </c>
+      <c r="C2" s="45">
+        <v>0.83932499999999999</v>
+      </c>
+      <c r="D2" s="45">
+        <v>0.86915299999999995</v>
+      </c>
+      <c r="E2" s="31">
+        <v>0.83770100000000003</v>
+      </c>
+      <c r="F2" s="32">
+        <v>0.82853900000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15" thickBot="1">
+      <c r="A3" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="42">
+        <v>0.86878500000000003</v>
+      </c>
+      <c r="C3" s="42">
+        <v>0.83852000000000004</v>
+      </c>
+      <c r="D3" s="42">
+        <v>0.86878500000000003</v>
+      </c>
+      <c r="E3" s="42">
+        <v>0.83710499999999999</v>
+      </c>
+      <c r="F3" s="36">
+        <v>0.82854099999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="44">
+        <v>0.86902100000000004</v>
+      </c>
+      <c r="C5" s="44">
+        <v>0.83910099999999999</v>
+      </c>
+      <c r="D5" s="44">
+        <v>0.86902100000000004</v>
+      </c>
+      <c r="E5" s="46">
+        <v>0.83774599999999999</v>
+      </c>
+      <c r="F5" s="38">
+        <v>0.82778499999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added thirteenth version of Jupyter notebook which adds neural network optimization; also included optimization log and notes
</commit_message>
<xml_diff>
--- a/Alex/Optimization_Metrics.xlsx
+++ b/Alex/Optimization_Metrics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asg_a_1p8y6mm\Downloads\Project_04\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECB0A5AD-654D-40DA-82EE-70D87E747AEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4EC97F5-4F60-4685-AACE-99C2BD1FCA47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{6E00537D-A3CB-4DE7-973B-44E1FD35F5BD}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="32">
   <si>
     <t>Accuracy</t>
   </si>
@@ -125,6 +125,12 @@
   </si>
   <si>
     <t>Logistic Regression 12 (Optimize Gradient Boosting; expanded with early stopping)</t>
+  </si>
+  <si>
+    <t>Neural Network</t>
+  </si>
+  <si>
+    <t>Logistic Regression 13 (Optimize Neural Network model)</t>
   </si>
 </sst>
 </file>
@@ -578,7 +584,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -624,26 +630,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -958,7 +966,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDBE8DC2-E395-4175-AFF2-1F4BE9386154}">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1242,22 +1250,22 @@
       <c r="A12" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="39" t="s">
+      <c r="B12" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="40">
+      <c r="C12" s="37">
         <v>0.86150499999999997</v>
       </c>
-      <c r="D12" s="40">
+      <c r="D12" s="37">
         <v>0.82802500000000001</v>
       </c>
-      <c r="E12" s="40">
+      <c r="E12" s="37">
         <v>0.86150499999999997</v>
       </c>
-      <c r="F12" s="40">
+      <c r="F12" s="37">
         <v>0.83425400000000005</v>
       </c>
-      <c r="G12" s="41">
+      <c r="G12" s="38">
         <v>0.80271800000000004</v>
       </c>
     </row>
@@ -1268,13 +1276,13 @@
       <c r="B13" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="45">
+      <c r="C13" s="41">
         <v>0.86915299999999995</v>
       </c>
-      <c r="D13" s="45">
+      <c r="D13" s="41">
         <v>0.83932499999999999</v>
       </c>
-      <c r="E13" s="45">
+      <c r="E13" s="41">
         <v>0.86915299999999995</v>
       </c>
       <c r="F13" s="31">
@@ -1285,10 +1293,10 @@
       </c>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="47" t="s">
+      <c r="A14" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="48" t="s">
+      <c r="B14" s="44" t="s">
         <v>25</v>
       </c>
       <c r="C14" s="5">
@@ -1303,35 +1311,87 @@
       <c r="F14" s="5">
         <v>0.83710499999999999</v>
       </c>
-      <c r="G14" s="49">
+      <c r="G14" s="45">
         <v>0.82854099999999997</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="15" thickBot="1">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="35" t="s">
+      <c r="B15" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="50">
+      <c r="C15" s="46">
         <v>0.86902100000000004</v>
       </c>
-      <c r="D15" s="50">
+      <c r="D15" s="46">
         <v>0.83910099999999999</v>
       </c>
-      <c r="E15" s="50">
+      <c r="E15" s="46">
         <v>0.86902100000000004</v>
       </c>
-      <c r="F15" s="33">
+      <c r="F15" s="37">
         <v>0.83774599999999999</v>
       </c>
-      <c r="G15" s="43">
+      <c r="G15" s="47">
         <v>0.82778499999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="37"/>
+    <row r="16" spans="1:9">
+      <c r="A16" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="49" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="31">
+        <v>0.86875899999999995</v>
+      </c>
+      <c r="D16" s="31">
+        <v>0.83781700000000003</v>
+      </c>
+      <c r="E16" s="31">
+        <v>0.86875899999999995</v>
+      </c>
+      <c r="F16" s="31">
+        <v>0.83255900000000005</v>
+      </c>
+      <c r="G16" s="32">
+        <v>0.82840599999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="48" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="5">
+        <v>0.86563100000000004</v>
+      </c>
+      <c r="D17" s="5">
+        <v>0.83261799999999997</v>
+      </c>
+      <c r="E17" s="5">
+        <v>0.86563100000000004</v>
+      </c>
+      <c r="F17" s="5">
+        <v>0.81212799999999996</v>
+      </c>
+      <c r="G17" s="11">
+        <v>0.82459899999999997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15" thickBot="1">
+      <c r="A18" s="50"/>
+      <c r="B18" s="33"/>
+      <c r="C18" s="51"/>
+      <c r="D18" s="51"/>
+      <c r="E18" s="51"/>
+      <c r="F18" s="51"/>
+      <c r="G18" s="52"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1377,13 +1437,13 @@
       <c r="A2" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="45">
+      <c r="B2" s="41">
         <v>0.86915299999999995</v>
       </c>
-      <c r="C2" s="45">
+      <c r="C2" s="41">
         <v>0.83932499999999999</v>
       </c>
-      <c r="D2" s="45">
+      <c r="D2" s="41">
         <v>0.86915299999999995</v>
       </c>
       <c r="E2" s="31">
@@ -1394,22 +1454,22 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" thickBot="1">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="42">
+      <c r="B3" s="39">
         <v>0.86878500000000003</v>
       </c>
-      <c r="C3" s="42">
+      <c r="C3" s="39">
         <v>0.83852000000000004</v>
       </c>
-      <c r="D3" s="42">
+      <c r="D3" s="39">
         <v>0.86878500000000003</v>
       </c>
-      <c r="E3" s="42">
+      <c r="E3" s="39">
         <v>0.83710499999999999</v>
       </c>
-      <c r="F3" s="36">
+      <c r="F3" s="34">
         <v>0.82854099999999997</v>
       </c>
     </row>
@@ -1417,19 +1477,19 @@
       <c r="A5" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="44">
+      <c r="B5" s="40">
         <v>0.86902100000000004</v>
       </c>
-      <c r="C5" s="44">
+      <c r="C5" s="40">
         <v>0.83910099999999999</v>
       </c>
-      <c r="D5" s="44">
+      <c r="D5" s="40">
         <v>0.86902100000000004</v>
       </c>
-      <c r="E5" s="46">
+      <c r="E5" s="42">
         <v>0.83774599999999999</v>
       </c>
-      <c r="F5" s="38">
+      <c r="F5" s="35">
         <v>0.82778499999999999</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated thirteenth version of Jupyter notebook as well as optimization log and notes
</commit_message>
<xml_diff>
--- a/Alex/Optimization_Metrics.xlsx
+++ b/Alex/Optimization_Metrics.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asg_a_1p8y6mm\Downloads\Project_04\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4EC97F5-4F60-4685-AACE-99C2BD1FCA47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E6750B8-C4FA-4DB8-BE54-E6DA63133B8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{6E00537D-A3CB-4DE7-973B-44E1FD35F5BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="29">
   <si>
     <t>Accuracy</t>
   </si>
@@ -109,19 +108,10 @@
     <t>Logistic Regression 10 (Optimize Random Forest)</t>
   </si>
   <si>
-    <t>Gradient</t>
-  </si>
-  <si>
     <t>Gradient Boosting</t>
   </si>
   <si>
     <t>Logistic Regression 11 (Optimize Gradient Boosting)</t>
-  </si>
-  <si>
-    <t>Before</t>
-  </si>
-  <si>
-    <t>After</t>
   </si>
   <si>
     <t>Logistic Regression 12 (Optimize Gradient Boosting; expanded with early stopping)</t>
@@ -140,7 +130,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -155,11 +145,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="5">
@@ -584,7 +569,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -631,27 +616,19 @@
     <xf numFmtId="164" fontId="0" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -966,11 +943,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDBE8DC2-E395-4175-AFF2-1F4BE9386154}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="81.36328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.453125" customWidth="1"/>
@@ -978,7 +955,7 @@
     <col min="9" max="9" width="24.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="15" thickBot="1">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="15" t="s">
         <v>5</v>
       </c>
@@ -1004,7 +981,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>11</v>
       </c>
@@ -1030,7 +1007,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>12</v>
       </c>
@@ -1056,7 +1033,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15" thickBot="1">
+    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="7" t="s">
         <v>13</v>
       </c>
@@ -1082,7 +1059,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15" thickBot="1">
+    <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="7" t="s">
         <v>14</v>
       </c>
@@ -1108,7 +1085,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>15</v>
       </c>
@@ -1131,7 +1108,7 @@
         <v>0.82350000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>16</v>
       </c>
@@ -1154,7 +1131,7 @@
         <v>0.82349300000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>17</v>
       </c>
@@ -1177,7 +1154,7 @@
         <v>0.82349300000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>18</v>
       </c>
@@ -1200,7 +1177,7 @@
         <v>0.82349300000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15" thickBot="1">
+    <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="25" t="s">
         <v>19</v>
       </c>
@@ -1223,7 +1200,7 @@
         <v>0.82349300000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="29" t="s">
         <v>19</v>
       </c>
@@ -1246,43 +1223,43 @@
         <v>0.79233299999999995</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15" thickBot="1">
+    <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="37">
+      <c r="C12" s="35">
         <v>0.86150499999999997</v>
       </c>
-      <c r="D12" s="37">
+      <c r="D12" s="35">
         <v>0.82802500000000001</v>
       </c>
-      <c r="E12" s="37">
+      <c r="E12" s="35">
         <v>0.86150499999999997</v>
       </c>
-      <c r="F12" s="37">
+      <c r="F12" s="35">
         <v>0.83425400000000005</v>
       </c>
-      <c r="G12" s="38">
+      <c r="G12" s="36">
         <v>0.80271800000000004</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="29" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="41">
+        <v>24</v>
+      </c>
+      <c r="C13" s="38">
         <v>0.86915299999999995</v>
       </c>
-      <c r="D13" s="41">
+      <c r="D13" s="38">
         <v>0.83932499999999999</v>
       </c>
-      <c r="E13" s="41">
+      <c r="E13" s="38">
         <v>0.86915299999999995</v>
       </c>
       <c r="F13" s="31">
@@ -1292,12 +1269,12 @@
         <v>0.82853900000000003</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="43" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="44" t="s">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" s="39" t="s">
         <v>25</v>
+      </c>
+      <c r="B14" s="40" t="s">
+        <v>24</v>
       </c>
       <c r="C14" s="5">
         <v>0.86878500000000003</v>
@@ -1311,189 +1288,81 @@
       <c r="F14" s="5">
         <v>0.83710499999999999</v>
       </c>
-      <c r="G14" s="45">
+      <c r="G14" s="41">
         <v>0.82854099999999997</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15" thickBot="1">
+    <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" s="36" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="46">
+        <v>26</v>
+      </c>
+      <c r="B15" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="42">
         <v>0.86902100000000004</v>
       </c>
-      <c r="D15" s="46">
+      <c r="D15" s="42">
         <v>0.83910099999999999</v>
       </c>
-      <c r="E15" s="46">
+      <c r="E15" s="42">
         <v>0.86902100000000004</v>
       </c>
-      <c r="F15" s="37">
+      <c r="F15" s="35">
         <v>0.83774599999999999</v>
       </c>
-      <c r="G15" s="47">
+      <c r="G15" s="43">
         <v>0.82778499999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="49" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="31">
+        <v>26</v>
+      </c>
+      <c r="B16" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="38">
         <v>0.86875899999999995</v>
       </c>
-      <c r="D16" s="31">
+      <c r="D16" s="38">
         <v>0.83781700000000003</v>
       </c>
-      <c r="E16" s="31">
+      <c r="E16" s="38">
         <v>0.86875899999999995</v>
       </c>
-      <c r="F16" s="31">
+      <c r="F16" s="38">
         <v>0.83255900000000005</v>
       </c>
-      <c r="G16" s="32">
+      <c r="G16" s="45">
         <v>0.82840599999999998</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="48" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="5">
+    <row r="17" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="44" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="37">
         <v>0.86563100000000004</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="37">
         <v>0.83261799999999997</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="37">
         <v>0.86563100000000004</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F17" s="37">
         <v>0.81212799999999996</v>
       </c>
-      <c r="G17" s="11">
+      <c r="G17" s="46">
         <v>0.82459899999999997</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="15" thickBot="1">
-      <c r="A18" s="50"/>
-      <c r="B18" s="33"/>
-      <c r="C18" s="51"/>
-      <c r="D18" s="51"/>
-      <c r="E18" s="51"/>
-      <c r="F18" s="51"/>
-      <c r="G18" s="52"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA0E0689-5345-46E6-81C6-E91955650508}">
-  <dimension ref="A1:F5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:F5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="1" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="8.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.54296875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1">
-      <c r="A1" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="41">
-        <v>0.86915299999999995</v>
-      </c>
-      <c r="C2" s="41">
-        <v>0.83932499999999999</v>
-      </c>
-      <c r="D2" s="41">
-        <v>0.86915299999999995</v>
-      </c>
-      <c r="E2" s="31">
-        <v>0.83770100000000003</v>
-      </c>
-      <c r="F2" s="32">
-        <v>0.82853900000000003</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15" thickBot="1">
-      <c r="A3" s="33" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" s="39">
-        <v>0.86878500000000003</v>
-      </c>
-      <c r="C3" s="39">
-        <v>0.83852000000000004</v>
-      </c>
-      <c r="D3" s="39">
-        <v>0.86878500000000003</v>
-      </c>
-      <c r="E3" s="39">
-        <v>0.83710499999999999</v>
-      </c>
-      <c r="F3" s="34">
-        <v>0.82854099999999997</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="40">
-        <v>0.86902100000000004</v>
-      </c>
-      <c r="C5" s="40">
-        <v>0.83910099999999999</v>
-      </c>
-      <c r="D5" s="40">
-        <v>0.86902100000000004</v>
-      </c>
-      <c r="E5" s="42">
-        <v>0.83774599999999999</v>
-      </c>
-      <c r="F5" s="35">
-        <v>0.82778499999999999</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>